<commit_message>
Added Account-Page, Contact-Page, Opportunity-page, and the flow is upto Opportunity Closed Lost
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestManager.xlsx
+++ b/src/test/resources/excel/TestManager.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VenkateshOrusu\Downloads\global-CRM-master\Keste_Salesforce\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_Project\Argano_Global_CRM\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDEDC7A-96EA-401D-B732-2A13D981D706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D16F0C-3814-49B5-AEA2-F64BE32D26F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="861" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>TestName</t>
   </si>
@@ -46,18 +46,9 @@
     <t>yes</t>
   </si>
   <si>
-    <t>CreateLeadAccount</t>
-  </si>
-  <si>
     <t>salesforce</t>
   </si>
   <si>
-    <t>CreateOpportunity</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -68,6 +59,12 @@
   </si>
   <si>
     <t>Venky@27</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -124,12 +121,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -414,7 +416,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -438,24 +440,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -469,7 +471,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E3"/>
+      <selection activeCell="F3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,15 +494,15 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -509,39 +511,37 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{C58B5714-E97D-43E0-B4F5-23E5768B0448}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{F60F5060-E66A-4991-A4F7-FB25E9CA6278}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{52891A24-0338-4CBE-B137-2532BBE06C42}"/>
-    <hyperlink ref="D2" r:id="rId4" xr:uid="{9719EF07-BE76-4A4F-BBBF-AFD275BBCCBE}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{9719EF07-BE76-4A4F-BBBF-AFD275BBCCBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -766,6 +766,28 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocIdPersistId xmlns="2f69742a-0218-4d1e-b734-635db9796963" xsi:nil="true"/>
+    <_dlc_DocId xmlns="2f69742a-0218-4d1e-b734-635db9796963">QPUHM6SRSPME-1180121400-1298</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="2f69742a-0218-4d1e-b734-635db9796963">
+      <Url>https://arganosolutions.sharepoint.com/sites/QARepository/_layouts/15/DocIdRedir.aspx?ID=QPUHM6SRSPME-1180121400-1298</Url>
+      <Description>QPUHM6SRSPME-1180121400-1298</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -815,28 +837,6 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocIdPersistId xmlns="2f69742a-0218-4d1e-b734-635db9796963" xsi:nil="true"/>
-    <_dlc_DocId xmlns="2f69742a-0218-4d1e-b734-635db9796963">QPUHM6SRSPME-1180121400-1298</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="2f69742a-0218-4d1e-b734-635db9796963">
-      <Url>https://arganosolutions.sharepoint.com/sites/QARepository/_layouts/15/DocIdRedir.aspx?ID=QPUHM6SRSPME-1180121400-1298</Url>
-      <Description>QPUHM6SRSPME-1180121400-1298</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35E16B5C-4DE3-49BB-934A-BDF63C97BB13}">
   <ds:schemaRefs>
@@ -857,22 +857,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C761976A-0385-4294-A9DF-BF78B934BC4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F44BF9C-5435-4768-B999-2A71E701C29F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{350DA447-2F7C-4D30-9DE9-76A24F0A2686}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -880,4 +864,20 @@
     <ds:schemaRef ds:uri="2f69742a-0218-4d1e-b734-635db9796963"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F44BF9C-5435-4768-B999-2A71E701C29F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C761976A-0385-4294-A9DF-BF78B934BC4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added the two methods in BasePage Class
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestManager.xlsx
+++ b/src/test/resources/excel/TestManager.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://arganosolutions-my.sharepoint.com/personal/akash_sv_argano_com/Documents/Framework Exection video/Argano CRM full  Regression script/ArganoGlobalCRM/src/test/resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_Project\Argano-Global-CRM\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{F2556545-4BC2-4CD7-8944-68779841E37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{994C6B66-3143-451C-A5C3-CBE0637CE09A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F171A29-0293-41C5-9F0A-F73996361C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="861" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="861" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -196,9 +196,6 @@
     <t>Prcomments</t>
   </si>
   <si>
-    <t>Akash SV</t>
-  </si>
-  <si>
     <t>LeadToClosedWon</t>
   </si>
   <si>
@@ -217,20 +214,23 @@
     <t>Verify validation When user tries to create customer account</t>
   </si>
   <si>
-    <t>akash.sv1@argano.com.full</t>
-  </si>
-  <si>
-    <t>Fenoy@2021</t>
-  </si>
-  <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>venkatesh.orusu1@argano.com.full</t>
+  </si>
+  <si>
+    <t>Venky@27</t>
+  </si>
+  <si>
+    <t>Venkatesh Orusu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,13 +276,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -317,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -334,10 +327,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -628,32 +617,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
         <v>61</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>
@@ -669,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A4785F-347E-4B80-9A39-C47650A76F4A}">
   <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -787,10 +776,10 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -798,7 +787,7 @@
       <c r="D2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="7" t="s">
         <v>64</v>
       </c>
       <c r="F2" t="s">
@@ -853,16 +842,16 @@
         <v>13</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="AA2" t="s">
         <v>14</v>
@@ -882,10 +871,10 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -977,7 +966,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
         <v>37</v>
@@ -1075,64 +1064,37 @@
   <hyperlinks>
     <hyperlink ref="R2" r:id="rId1" xr:uid="{D1643F92-5818-4242-99F1-060031DBC663}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{DE6C321A-9C16-43DB-8C53-7F288C33F737}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{774444FF-AC0B-4DFA-BD10-A80B2CB93C03}"/>
+    <hyperlink ref="D3:D4" r:id="rId3" display="venkatesh.orusu1@argano.com.full" xr:uid="{2094EAFB-AF4B-450A-8657-E2D3AF1FECFA}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{0B0573C1-2AE1-4516-969A-2DA6CF8ADC64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocIdPersistId xmlns="2f69742a-0218-4d1e-b734-635db9796963" xsi:nil="true"/>
+    <_dlc_DocId xmlns="2f69742a-0218-4d1e-b734-635db9796963">QPUHM6SRSPME-1180121400-1298</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="2f69742a-0218-4d1e-b734-635db9796963">
+      <Url>https://arganosolutions.sharepoint.com/sites/QARepository/_layouts/15/DocIdRedir.aspx?ID=QPUHM6SRSPME-1180121400-1298</Url>
+      <Description>QPUHM6SRSPME-1180121400-1298</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010069379168F6D42B4E9BAD3B7EA681D21F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="02753efbd18866d629148b62e97d7453">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2f69742a-0218-4d1e-b734-635db9796963" xmlns:ns3="a199da25-74a0-4b1e-a49c-2c847b028b82" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9bdac05109f73751124109d61ff8f9b5" ns2:_="" ns3:_="">
     <xsd:import namespace="2f69742a-0218-4d1e-b734-635db9796963"/>
@@ -1352,37 +1314,75 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocIdPersistId xmlns="2f69742a-0218-4d1e-b734-635db9796963" xsi:nil="true"/>
-    <_dlc_DocId xmlns="2f69742a-0218-4d1e-b734-635db9796963">QPUHM6SRSPME-1180121400-1298</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="2f69742a-0218-4d1e-b734-635db9796963">
-      <Url>https://arganosolutions.sharepoint.com/sites/QARepository/_layouts/15/DocIdRedir.aspx?ID=QPUHM6SRSPME-1180121400-1298</Url>
-      <Description>QPUHM6SRSPME-1180121400-1298</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C761976A-0385-4294-A9DF-BF78B934BC4A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F44BF9C-5435-4768-B999-2A71E701C29F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{350DA447-2F7C-4D30-9DE9-76A24F0A2686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2f69742a-0218-4d1e-b734-635db9796963"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35E16B5C-4DE3-49BB-934A-BDF63C97BB13}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1401,20 +1401,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{350DA447-2F7C-4D30-9DE9-76A24F0A2686}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C761976A-0385-4294-A9DF-BF78B934BC4A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2f69742a-0218-4d1e-b734-635db9796963"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F44BF9C-5435-4768-B999-2A71E701C29F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>